<commit_message>
updated lookup table for OEKS15 time lag
</commit_message>
<xml_diff>
--- a/data/gwl_lists/Gaps_rwl_gwl10_OEKS15_lookup_table.xlsx
+++ b/data/gwl_lists/Gaps_rwl_gwl10_OEKS15_lookup_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbecsi/Desktop/Arbeit/Qgis/data/AAR2/GWLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3A1ABD-A68C-594F-AEF6-12427256B2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19BCA83-AF16-B944-8CD1-5DDD5FB2781B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21860" xr2:uid="{F9128DBB-4346-C142-AB1F-4CECC8BAD8E6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>Period</t>
   </si>
@@ -44,15 +44,9 @@
     <t>CNRM-CERFACS-CNRM-CM5_rcp45_r1i1p1_CLMcom-CCLM4-8-17</t>
   </si>
   <si>
-    <t>2044-2063</t>
-  </si>
-  <si>
     <t>CNRM-CERFACS-CNRM-CM5_rcp45_r1i1p1_CNRM-ALADIN53</t>
   </si>
   <si>
-    <t>2018-2037</t>
-  </si>
-  <si>
     <t>CNRM-CERFACS-CNRM-CM5_rcp45_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
@@ -62,15 +56,9 @@
     <t>CNRM-CERFACS-CNRM-CM5_rcp85_r1i1p1_CLMcom-CCLM4-8-17</t>
   </si>
   <si>
-    <t>2033-2052</t>
-  </si>
-  <si>
     <t>CNRM-CERFACS-CNRM-CM5_rcp85_r1i1p1_CNRM-ALADIN53</t>
   </si>
   <si>
-    <t>2014-2033</t>
-  </si>
-  <si>
     <t>CNRM-CERFACS-CNRM-CM5_rcp85_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
@@ -89,15 +77,9 @@
     <t>ICHEC-EC-EARTH_rcp26_r12i1p1_SMHI-RCA4</t>
   </si>
   <si>
-    <t>2023-2042</t>
-  </si>
-  <si>
     <t>ICHEC-EC-EARTH_rcp26_r3i1p1_DMI-HIRHAM5</t>
   </si>
   <si>
-    <t>2039-2058</t>
-  </si>
-  <si>
     <t>ICHEC-EC-EARTH_rcp45_r12i1p1_CLMcom-CCLM4-8-17</t>
   </si>
   <si>
@@ -140,33 +122,18 @@
     <t>IPSL-IPSL-CM5A-MR_rcp45_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
-    <t>2015-2034</t>
-  </si>
-  <si>
     <t>IPSL-IPSL-CM5A-MR_rcp85_r1i1p1_IPSL-INERIS-WRF331F</t>
   </si>
   <si>
-    <t>1999-2018</t>
-  </si>
-  <si>
     <t>IPSL-IPSL-CM5A-MR_rcp85_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
-    <t>2003-2022</t>
-  </si>
-  <si>
     <t>MOHC-HadGEM2-ES_rcp26_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
-    <t>2004-2023</t>
-  </si>
-  <si>
     <t>MOHC-HadGEM2-ES_rcp45_r1i1p1_CLMcom-CCLM4-8-17</t>
   </si>
   <si>
-    <t>2007-2026</t>
-  </si>
-  <si>
     <t>MOHC-HadGEM2-ES_rcp45_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
@@ -179,15 +146,9 @@
     <t>MOHC-HadGEM2-ES_rcp85_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
-    <t>2002-2021</t>
-  </si>
-  <si>
     <t>MPI-M-MPI-ESM-LR_rcp26_r1i1p1_MPI-CSC-REMO2009</t>
   </si>
   <si>
-    <t>2062-2081</t>
-  </si>
-  <si>
     <t>MPI-M-MPI-ESM-LR_rcp26_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
@@ -203,28 +164,52 @@
     <t>MPI-M-MPI-ESM-LR_rcp45_r1i1p1_CLMcom-CCLM4-8-17</t>
   </si>
   <si>
-    <t>2046-2065</t>
-  </si>
-  <si>
     <t>MPI-M-MPI-ESM-LR_rcp45_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
     <t>MPI-M-MPI-ESM-LR_rcp85_r1i1p1_CLMcom-CCLM4-8-17</t>
   </si>
   <si>
-    <t>2032-2051</t>
-  </si>
-  <si>
     <t>MPI-M-MPI-ESM-LR_rcp85_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
-    <t>2024-2043</t>
-  </si>
-  <si>
     <t>Gap (Years)</t>
   </si>
   <si>
     <t>Period when models reach observed warming of SPARTACUS between 1971-2000 and GWL1.0 (2001-2020)</t>
+  </si>
+  <si>
+    <t>2045-2064</t>
+  </si>
+  <si>
+    <t>2036-2055</t>
+  </si>
+  <si>
+    <t>2027-2046</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>2041-2060</t>
+  </si>
+  <si>
+    <t>2026-2045</t>
+  </si>
+  <si>
+    <t>2030-2049</t>
+  </si>
+  <si>
+    <t>2017-2036</t>
+  </si>
+  <si>
+    <t>2001-2020</t>
+  </si>
+  <si>
+    <t>2008-2027</t>
+  </si>
+  <si>
+    <t>2019-2038</t>
   </si>
 </sst>
 </file>
@@ -599,7 +584,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,13 +595,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -624,133 +609,139 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="C2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C5">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="C7">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <v>28</v>
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C12">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C13">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>19</v>
@@ -758,43 +749,43 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15">
         <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C16">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C17">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>9</v>
@@ -802,21 +793,21 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C19">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>20</v>
@@ -824,76 +815,76 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C21">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C22">
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -901,90 +892,90 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="C29">
-        <v>61</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C30">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31">
-        <v>5</v>
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="C32">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C33">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="C34">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>